<commit_message>
Worked and completed Email Functionality
</commit_message>
<xml_diff>
--- a/automationtraining/src/test/java/testdata.xlsx
+++ b/automationtraining/src/test/java/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3A45B0B9-6440-4DAA-B6E4-E1F381C9D159}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{86ADCFA0-FF69-4361-823D-882F13E30C51}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="5835" xr2:uid="{221D4FD3-E661-4E3B-8080-3B00F72440CB}"/>
   </bookViews>
@@ -16,12 +16,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -197,9 +191,6 @@
     <t>01-05-2012</t>
   </si>
   <si>
-    <t>sindhube@gmail.com</t>
-  </si>
-  <si>
     <t>submitteremail</t>
   </si>
   <si>
@@ -207,16 +198,27 @@
   </si>
   <si>
     <t>TCAT_101</t>
+  </si>
+  <si>
+    <t>sindhuja.e@mstsolutions.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -239,15 +241,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -562,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44D3B42-8979-4DAD-92A6-CDE1B767810B}">
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AD6" sqref="AD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +604,7 @@
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -707,12 +712,12 @@
         <v>54</v>
       </c>
       <c r="AK1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -819,11 +824,14 @@
       <c r="AJ2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AK2" t="s">
-        <v>56</v>
+      <c r="AK2" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AK2" r:id="rId1" xr:uid="{4977F9FA-CBEB-43AE-BD52-4F552554B344}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>